<commit_message>
var decisions tn tp
</commit_message>
<xml_diff>
--- a/Benchmarks/Water Chemistry/Total Phosphorus/Var selection decisions 1-22-26.xlsx
+++ b/Benchmarks/Water Chemistry/Total Phosphorus/Var selection decisions 1-22-26.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/adam_thompson_deq_oregon_gov/Documents/Documents/BioMonORDEQ/Benchmarks/Water Chemistry/Total Phosphorus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{6B8D232A-EEA6-4563-A1A6-87C6EEBA49F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB08D7E5-1148-40EA-AAB8-4799F2FB030F}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="8_{6B8D232A-EEA6-4563-A1A6-87C6EEBA49F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A4B5E-C3EA-4BD4-BE7A-9603F9560709}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30624" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="234">
   <si>
     <t>num_vars</t>
   </si>
@@ -459,9 +459,6 @@
     <t>WWTPMINORDENSWS</t>
   </si>
   <si>
-    <t>Keep or remove</t>
-  </si>
-  <si>
     <t>Rationale</t>
   </si>
   <si>
@@ -592,13 +589,205 @@
   </si>
   <si>
     <t>neg - more permeable soils will capture more n/p?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Keep or remove</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Keep or remove</t>
+    </r>
+  </si>
+  <si>
+    <t>REMOVE</t>
+  </si>
+  <si>
+    <t>distribution not as good as others</t>
+  </si>
+  <si>
+    <t>KEEP</t>
+  </si>
+  <si>
+    <t>slightly better distribution, more direct measure</t>
+  </si>
+  <si>
+    <t>Captured in KFFACT which wasn't correlated with anything, kept in favor of fert</t>
+  </si>
+  <si>
+    <t>favored direct measure of phos oxide</t>
+  </si>
+  <si>
+    <t>direct measure for P</t>
+  </si>
+  <si>
+    <t>wanted to use a N metric (NANI or NSURP)</t>
+  </si>
+  <si>
+    <t>lots of metrics, easier to explain</t>
+  </si>
+  <si>
+    <t>worse CV than NANI, harder to explain</t>
+  </si>
+  <si>
+    <t>related to nutrients via gw inputs</t>
+  </si>
+  <si>
+    <t>doesn't make predictions everywhere, opted for baseflow</t>
+  </si>
+  <si>
+    <t>good distribution, better than others</t>
+  </si>
+  <si>
+    <t>chose baseflow</t>
+  </si>
+  <si>
+    <t>not permeable, so nutrients likely to runoff, better distribution than perm</t>
+  </si>
+  <si>
+    <t>better distribution on clay, inversely related</t>
+  </si>
+  <si>
+    <t>chose other dam metrics</t>
+  </si>
+  <si>
+    <t>normal storage preferred over max (NID) storage as better indication of normal conditions</t>
+  </si>
+  <si>
+    <t>chose normal storage</t>
+  </si>
+  <si>
+    <t>not as explainable for nutrients as storage</t>
+  </si>
+  <si>
+    <t>good general representation of other factors, good spread</t>
+  </si>
+  <si>
+    <t>kept elev</t>
+  </si>
+  <si>
+    <t>chose Fe since higher CV</t>
+  </si>
+  <si>
+    <t>slightly higher CV over Si, used in some ag fertilizers</t>
+  </si>
+  <si>
+    <t>chose population density</t>
+  </si>
+  <si>
+    <t>simpler than housing density, very similar distributions</t>
+  </si>
+  <si>
+    <t>single measure, chose inorganicwetdep since it encompassed this</t>
+  </si>
+  <si>
+    <t>liked inorganic wetdep better, almost 1:1 correlation</t>
+  </si>
+  <si>
+    <t>direct measure and gets at precip since metric is weighted</t>
+  </si>
+  <si>
+    <t>didn't want to use N metric for P, so chose a precip metric</t>
+  </si>
+  <si>
+    <t>liked precip minus evt</t>
+  </si>
+  <si>
+    <t>kept precip_evt for P</t>
+  </si>
+  <si>
+    <t>kept due to cascading dependencies and wanted precip evt</t>
+  </si>
+  <si>
+    <t>kept phos oxide</t>
+  </si>
+  <si>
+    <t>easier to understand, slightly better CV</t>
+  </si>
+  <si>
+    <t>kept erod</t>
+  </si>
+  <si>
+    <t>easier to understand, fewer zeros</t>
+  </si>
+  <si>
+    <t>kept hay</t>
+  </si>
+  <si>
+    <t>kept %burnarea</t>
+  </si>
+  <si>
+    <t>more general than other more specific metrics, mean over long timespan</t>
+  </si>
+  <si>
+    <t>kept general</t>
+  </si>
+  <si>
+    <t>general imperv easier to explain, distributions similar, fewer zeros</t>
+  </si>
+  <si>
+    <t>slightly better than mid</t>
+  </si>
+  <si>
+    <t>kept low urb</t>
+  </si>
+  <si>
+    <t>better anchored in time for reference condition</t>
+  </si>
+  <si>
+    <t>selected to be consistent w/ cond</t>
+  </si>
+  <si>
+    <t>dropped in favor of all</t>
+  </si>
+  <si>
+    <t>more general</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +806,14 @@
     <font>
       <strike/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -649,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,19 +858,122 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -994,908 +1294,1584 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="59.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="B27" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" t="s">
+        <v>212</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" t="s">
+        <v>192</v>
+      </c>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" t="s">
+        <v>220</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" t="s">
+        <v>223</v>
+      </c>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" t="s">
+        <v>225</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67" t="s">
+        <v>224</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="7"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70" s="9"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D71" s="7"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71" s="9"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="7"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72" s="9"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="7"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>188</v>
+      </c>
+      <c r="C75" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" t="s">
+        <v>222</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" t="s">
+        <v>188</v>
+      </c>
+      <c r="D80" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" t="s">
+        <v>186</v>
+      </c>
+      <c r="D81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>186</v>
+      </c>
+      <c r="C84" t="s">
+        <v>186</v>
+      </c>
+      <c r="D84" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="s">
+        <v>186</v>
+      </c>
+      <c r="D85" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" t="s">
+        <v>186</v>
+      </c>
+      <c r="D86" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" t="s">
+        <v>186</v>
+      </c>
+      <c r="D88" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" t="s">
+        <v>186</v>
+      </c>
+      <c r="D93" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" t="s">
+        <v>186</v>
+      </c>
+      <c r="D94" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D95" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E95" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D96" s="10"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" t="s">
+        <v>188</v>
+      </c>
+      <c r="D96" t="s">
+        <v>228</v>
+      </c>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D97" s="10"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" t="s">
+        <v>186</v>
+      </c>
+      <c r="D97" t="s">
+        <v>229</v>
+      </c>
+      <c r="E97" s="8"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D98" s="10"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" t="s">
+        <v>186</v>
+      </c>
+      <c r="D101" t="s">
+        <v>201</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E102" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>188</v>
+      </c>
+      <c r="C103" t="s">
+        <v>188</v>
+      </c>
+      <c r="D103" t="s">
+        <v>211</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104" t="s">
+        <v>186</v>
+      </c>
+      <c r="D104" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>186</v>
+      </c>
+      <c r="C105" t="s">
+        <v>186</v>
+      </c>
+      <c r="D105" t="s">
+        <v>216</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D106" s="7"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>186</v>
+      </c>
+      <c r="C106" t="s">
+        <v>186</v>
+      </c>
+      <c r="D106" t="s">
+        <v>216</v>
+      </c>
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D107" s="7"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>186</v>
+      </c>
+      <c r="C107" t="s">
+        <v>186</v>
+      </c>
+      <c r="D107" t="s">
+        <v>216</v>
+      </c>
+      <c r="E107" s="9"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E108" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D109" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E109" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D110" s="8"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E110" s="10"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D111" s="8"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E111" s="10"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E112" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>186</v>
+      </c>
+      <c r="C113" t="s">
+        <v>186</v>
+      </c>
+      <c r="D113" t="s">
+        <v>217</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E116" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>186</v>
+      </c>
+      <c r="C117" t="s">
+        <v>186</v>
+      </c>
+      <c r="D117" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" t="s">
+        <v>186</v>
+      </c>
+      <c r="D118" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>188</v>
+      </c>
+      <c r="C121" t="s">
+        <v>188</v>
+      </c>
+      <c r="D121" t="s">
+        <v>218</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="9" t="s">
+      <c r="E122" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>186</v>
+      </c>
+      <c r="C124" t="s">
+        <v>186</v>
+      </c>
+      <c r="D124" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D125" s="7"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>186</v>
+      </c>
+      <c r="C125" t="s">
+        <v>186</v>
+      </c>
+      <c r="D125" t="s">
+        <v>230</v>
+      </c>
+      <c r="E125" s="9"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D126" s="7"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>188</v>
+      </c>
+      <c r="C126" t="s">
+        <v>188</v>
+      </c>
+      <c r="D126" t="s">
+        <v>231</v>
+      </c>
+      <c r="E126" s="9"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="7"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>186</v>
+      </c>
+      <c r="C127" t="s">
+        <v>186</v>
+      </c>
+      <c r="D127" t="s">
+        <v>199</v>
+      </c>
+      <c r="E127" s="9"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D128" s="7"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C128" t="s">
+        <v>186</v>
+      </c>
+      <c r="D128" t="s">
+        <v>199</v>
+      </c>
+      <c r="E128" s="9"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D129" s="7"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>186</v>
+      </c>
+      <c r="C129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D129" t="s">
+        <v>199</v>
+      </c>
+      <c r="E129" s="9"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D130" s="7"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>186</v>
+      </c>
+      <c r="C130" t="s">
+        <v>186</v>
+      </c>
+      <c r="D130" t="s">
+        <v>199</v>
+      </c>
+      <c r="E130" s="9"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D131" s="7"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>186</v>
+      </c>
+      <c r="C131" t="s">
+        <v>186</v>
+      </c>
+      <c r="D131" t="s">
+        <v>199</v>
+      </c>
+      <c r="E131" s="9"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>186</v>
+      </c>
+      <c r="C133" t="s">
+        <v>186</v>
+      </c>
+      <c r="D133" t="s">
+        <v>187</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>186</v>
+      </c>
+      <c r="C134" t="s">
+        <v>186</v>
+      </c>
+      <c r="D134" t="s">
+        <v>187</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>186</v>
+      </c>
+      <c r="C136" t="s">
+        <v>186</v>
+      </c>
+      <c r="D136" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D138" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>188</v>
+      </c>
+      <c r="C138" t="s">
+        <v>188</v>
+      </c>
+      <c r="D138" t="s">
+        <v>233</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D139" s="7"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E139" s="9"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D140" s="7"/>
+      <c r="B140" t="s">
+        <v>186</v>
+      </c>
+      <c r="C140" t="s">
+        <v>186</v>
+      </c>
+      <c r="D140" t="s">
+        <v>232</v>
+      </c>
+      <c r="E140" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D140" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E140" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="10">
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="D138:D140"/>
-    <mergeCell ref="D125:D131"/>
-    <mergeCell ref="D109:D111"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D95:D98"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E69:E73"/>
+    <mergeCell ref="E105:E107"/>
+    <mergeCell ref="E138:E140"/>
+    <mergeCell ref="E125:E131"/>
+    <mergeCell ref="E109:E111"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E95:E98"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B140">
+  <conditionalFormatting sqref="C2:C74 C76:C79 C81:C112 C114:C140">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"KEEP"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="REMOVE">
+      <formula>NOT(ISERROR(SEARCH("REMOVE",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B103 B105:B140">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"KEEP"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="REMOVE">
+      <formula>NOT(ISERROR(SEARCH("REMOVE",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B104">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"KEEP"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="REMOVE">
+      <formula>NOT(ISERROR(SEARCH("REMOVE",B104)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C113">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"KEEP"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="REMOVE">
+      <formula>NOT(ISERROR(SEARCH("REMOVE",C113)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"KEEP"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="REMOVE">
+      <formula>NOT(ISERROR(SEARCH("REMOVE",C75)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"KEEP"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("REMOVE",C80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B140" xr:uid="{EB42C186-6836-4773-A6E5-B88EA86420AD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C140" xr:uid="{EB42C186-6836-4773-A6E5-B88EA86420AD}">
       <formula1>"KEEP, REMOVE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1927,7 +2903,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TP model builds w/ Sabiney.
</commit_message>
<xml_diff>
--- a/Benchmarks/Water Chemistry/Total Phosphorus/Var selection decisions 1-22-26.xlsx
+++ b/Benchmarks/Water Chemistry/Total Phosphorus/Var selection decisions 1-22-26.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/adam_thompson_deq_oregon_gov/Documents/Documents/BioMonORDEQ/Benchmarks/Water Chemistry/Total Phosphorus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{6B8D232A-EEA6-4563-A1A6-87C6EEBA49F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A4B5E-C3EA-4BD4-BE7A-9603F9560709}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="8_{6B8D232A-EEA6-4563-A1A6-87C6EEBA49F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{484C1EF8-3A8D-41F5-881E-160E3906B7A3}"/>
   <bookViews>
-    <workbookView xWindow="30624" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47748" yWindow="0" windowWidth="13788" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$140</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="234">
   <si>
     <t>num_vars</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>Ecological Perspective</t>
-  </si>
-  <si>
-    <t>BFIWS, CANALDENSWS, CAOWS, CLAYWS, COMPSTRGTHWS, DAMDENSWS, ELEVWS, FE2O3WS, HYDRLCONDWS, K2OWS, KFFACTWS, MINEDENSWS, MSST2008, NA2OWS, NHD_pSLOPE, NPDESDENSWS, NWS, OMWS, PCT_EROD, PCTAGDRAINAGEWS, PCTAGSLPMID2001WS, PCTALKINTRUVOLWS, PCTALLUVCOASTWS, PCTBL2001WS, PCTBURNAREA2002WS, PCTCOLLUVSEDWS, PCTCONIF2001WS, PCTCROP2001WS, PCTDECID2001WS, PCTEOLCRSWS, PCTEOLFINEWS, PCTEXTRUVOLWS, PCTFRSTLOSS2002WS, PCTGLACLAKECRSWS, PCTGLACLAKEFINEWS, PCTGLACTILCRSWS, PCTGRS2001WS, PCTHBWET2001WS, PCTICE2001WS, PCTIMP2001WS, PCTINCVEGRESP2002WS, PCTNONAGINTRODMANAGVEGWS, PCTOW2001WS, PCTSALLAKEWS, PCTSHRB2001WS, PCTURBHI2001WS, PCTURBLO2001WS, PCTURBOP2001WS, PCTWATERWS, PESTIC1997WS, POPDEN2010WS, PRECIP9120WS, RCKDEPWS, RDCRSSLPWTDWS, RDCRSWS, RDDENSWS, ROCKNWS, SANDWS, SEPTICWS, STRMPOW_CAT, SUPERFUNDDENSWS, SW_FLUXWS, SWS, TMAX9120WS, TRIDENSWS, WATERINPUTWS, WETINDEXWS, WETTEDWIDTH, WTDEPWS, WWTPALLDENSWS</t>
   </si>
   <si>
     <t>pos - more fert more nutrients</t>
@@ -781,6 +778,9 @@
   </si>
   <si>
     <t>more general</t>
+  </si>
+  <si>
+    <t>all 0s</t>
   </si>
 </sst>
 </file>
@@ -859,6 +859,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -866,114 +869,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1294,30 +1194,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E140"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="59.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="37.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>140</v>
@@ -1326,1490 +1227,1619 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
         <v>186</v>
       </c>
-      <c r="C9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" t="s">
-        <v>187</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" t="s">
         <v>188</v>
       </c>
-      <c r="C21" t="s">
-        <v>188</v>
-      </c>
-      <c r="D21" t="s">
-        <v>189</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" t="s">
         <v>186</v>
       </c>
-      <c r="C31" t="s">
-        <v>186</v>
-      </c>
-      <c r="D31" t="s">
-        <v>187</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D33" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s">
-        <v>202</v>
-      </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
-      </c>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D49" t="s">
-        <v>192</v>
-      </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C52" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D52" t="s">
-        <v>223</v>
-      </c>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
-      </c>
-      <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E69" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E71" s="9"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" t="s">
+        <v>233</v>
+      </c>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E72" s="9"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E73" s="9"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>185</v>
+      </c>
+      <c r="C73" t="s">
+        <v>185</v>
+      </c>
+      <c r="D73" t="s">
+        <v>233</v>
+      </c>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D75" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D77" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>185</v>
+      </c>
+      <c r="C78" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D80" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D81" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D82" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C84" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D84" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C85" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D85" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D86" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D88" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" t="s">
+        <v>185</v>
+      </c>
+      <c r="D89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C93" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D93" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D94" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E95" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D96" t="s">
-        <v>228</v>
-      </c>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+      <c r="E96" s="9"/>
+    </row>
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D97" t="s">
-        <v>229</v>
-      </c>
-      <c r="E97" s="8"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+      <c r="E97" s="9"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E98" s="8"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E98" s="9"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C101" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>101</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C103" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C104" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D104" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C105" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D105" t="s">
-        <v>216</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D106" t="s">
-        <v>216</v>
-      </c>
-      <c r="E106" s="9"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="E106" s="10"/>
+    </row>
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C107" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D107" t="s">
-        <v>216</v>
-      </c>
-      <c r="E107" s="9"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E109" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E109" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E110" s="10"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E110" s="11"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E111" s="10"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E111" s="11"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C113" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D113" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>185</v>
+      </c>
+      <c r="C115" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C117" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D117" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C118" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D118" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C121" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D121" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>185</v>
+      </c>
+      <c r="C123" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C124" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D124" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D125" t="s">
-        <v>230</v>
-      </c>
-      <c r="E125" s="9"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+      <c r="E125" s="10"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C126" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D126" t="s">
-        <v>231</v>
-      </c>
-      <c r="E126" s="9"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+      <c r="E126" s="10"/>
+    </row>
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C127" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D127" t="s">
-        <v>199</v>
-      </c>
-      <c r="E127" s="9"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E127" s="10"/>
+    </row>
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C128" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D128" t="s">
-        <v>199</v>
-      </c>
-      <c r="E128" s="9"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E128" s="10"/>
+    </row>
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D129" t="s">
-        <v>199</v>
-      </c>
-      <c r="E129" s="9"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E129" s="10"/>
+    </row>
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D130" t="s">
-        <v>199</v>
-      </c>
-      <c r="E130" s="9"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E130" s="10"/>
+    </row>
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C131" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D131" t="s">
-        <v>199</v>
-      </c>
-      <c r="E131" s="9"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B133" t="s">
+        <v>185</v>
+      </c>
+      <c r="C133" t="s">
+        <v>185</v>
+      </c>
+      <c r="D133" t="s">
         <v>186</v>
       </c>
-      <c r="C133" t="s">
-        <v>186</v>
-      </c>
-      <c r="D133" t="s">
-        <v>187</v>
-      </c>
       <c r="E133" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B134" t="s">
+        <v>185</v>
+      </c>
+      <c r="C134" t="s">
+        <v>185</v>
+      </c>
+      <c r="D134" t="s">
         <v>186</v>
       </c>
-      <c r="C134" t="s">
-        <v>186</v>
-      </c>
-      <c r="D134" t="s">
-        <v>187</v>
-      </c>
       <c r="E134" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C136" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D136" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C138" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D138" t="s">
-        <v>233</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+      <c r="E138" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E139" s="9"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E139" s="10"/>
+    </row>
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C140" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D140" t="s">
-        <v>232</v>
-      </c>
-      <c r="E140" s="9"/>
+        <v>231</v>
+      </c>
+      <c r="E140" s="10"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" t="str">
+        <f>_xlfn.TEXTJOIN(", ", TRUE, A2:A139)</f>
+        <v>AGKFFACTWS, AL2O3WS, BANKFULLDEPTH, BANKFULLWIDTH, BFIWS, CANALDENSWS, CAOWS, CBNFWS, CHEMWS, CLAYWS, COALMINEDENSWS, COMID, COMPSTRGTHWS, CONNWS, DAMDENSWS, DAMNIDSTORWS, DAMNRMSTORWS, ELEVWS, FE2O3WS, FERTWS, HABTWS, HUDEN2010WS, HYDRLCONDWS, HYDWS, ICI, INORGNWETDEP2008WS, IWI, K2OWS, KFFACTWS, MANUREWS, MAST2008, MGOWS, MINEDENSWS, MSST2008, MWST2008, NA2OWS, NABD_DENSWS, NABD_NIDSTORWS, NABD_NRMSTORWS, NANIWS, NH42008WS, NHD_pSLOPE, NO32008WS, NPDESDENSWS, NSURPWS, NWS, OMWS, P2O5WS, PCT_EROD, PCTAGDRAINAGEWS, PCTAGSLPHIGH2001WS, PCTAGSLPMID2001WS, PCTALKINTRUVOLWS, PCTALLUVCOASTWS, PCTBL2001WS, PCTBURNAREA2002WS, PCTCARBRESIDWS, PCTCOASTCRSWS, PCTCOLLUVSEDWS, PCTCONIF2001WS, PCTCROP2001WS, PCTDECID2001WS, PCTEOLCRSWS, PCTEOLFINEWS, PCTEXTRUVOLWS, PCTFIRE2002WS, PCTFRSTLOSS2002WS, PCTGLACLAKECRSWS, PCTGLACLAKEFINEWS, PCTGLACTILCLAYWS, PCTGLACTILCRSWS, PCTGLACTILLOAMWS, PCTGRS2001WS, PCTHAY2001WS, PCTHBWET2001WS, PCTHIGHSEV2002WS, PCTHYDRICWS, PCTICE2001WS, PCTIMP2001WS, PCTIMPSLPHIGH2001WS, PCTIMPSLPMID2001WS, PCTINCVEGRESP2002WS, PCTLOWSEV2002WS, PCTMODSEV2002WS, PCTMXFST2001WS, PCTNONAGINTRODMANAGVEGWS, PCTNONCARBRESIDWS, PCTNONPROCMASK2002WS, PCTOW2001WS, PCTSALLAKEWS, PCTSHRB2001WS, PCTSILICICWS, PCTUNDSEV2002WS, PCTURBHI2001WS, PCTURBLO2001WS, PCTURBMD2001WS, PCTURBOP2001WS, PCTWATERWS, PCTWDWET2001WS, PERMWS, PESTIC1997WS, POPDEN2010WS, PRECIP_MINUS_EVTWS, PRECIP2008WS, PRECIP8110WS, PRECIP9120WS, RCKDEPWS, RDCRSSLPWTDWS, RDCRSWS, RDDENSWS, ROCKNWS, RUNOFFWS, SANDWS, SEDWS, SEPTICWS, SIO2WS, SN2008WS, STRMPOW_CAT, SUPERFUNDDENSWS, SW_FLUXWS, SWS, TEMPWS, THALWEGDEPTH, TMAX8110WS, TMAX9120WS, TMEAN2008WS, TMEAN8110WS, TMEAN9120WS, TMIN8110WS, TMIN9120WS, TRIDENSWS, WATERINPUTWS, WDRW_LDWS, WETINDEXWS, WETTEDWIDTH, WTDEPWS, WWTPALLDENSWS, WWTPMAJORDENSWS</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E140" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E140" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters blank="1">
+        <filter val="KEEP"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="10">
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="E69:E73"/>
@@ -2822,55 +2852,15 @@
     <mergeCell ref="E38:E40"/>
     <mergeCell ref="E95:E98"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C74 C76:C79 C81:C112 C114:C140">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"KEEP"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B103 B105:B140">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"KEEP"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"KEEP"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",B104)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"KEEP"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",C113)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"KEEP"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",C75)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
+  <conditionalFormatting sqref="D12 B60:C63 B59:D59 B65:C70 B64:D64 B72:C72 B71:D71 B74:C77 B73:D73 B79:C88 B78:D78 B89:D89 B2:C58 B90:C140">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"KEEP"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="REMOVE">
-      <formula>NOT(ISERROR(SEARCH("REMOVE",C80)))</formula>
+      <formula>NOT(ISERROR(SEARCH("REMOVE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C140" xr:uid="{EB42C186-6836-4773-A6E5-B88EA86420AD}">
       <formula1>"KEEP, REMOVE"</formula1>
     </dataValidation>
@@ -2880,370 +2870,374 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436B77FA-BCAA-44EA-8D79-399215CFE77B}">
-  <dimension ref="A1:D70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077211B4-8B56-4334-A6B9-B5C347A0B98D}">
+  <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, A:A)</f>
-        <v>BFIWS, CANALDENSWS, CAOWS, CLAYWS, COMPSTRGTHWS, DAMDENSWS, ELEVWS, FE2O3WS, HYDRLCONDWS, K2OWS, KFFACTWS, MINEDENSWS, MSST2008, NA2OWS, NHD_pSLOPE, NPDESDENSWS, NWS, OMWS, PCT_EROD, PCTAGDRAINAGEWS, PCTAGSLPMID2001WS, PCTALKINTRUVOLWS, PCTALLUVCOASTWS, PCTBL2001WS, PCTBURNAREA2002WS, PCTCOLLUVSEDWS, PCTCONIF2001WS, PCTCROP2001WS, PCTDECID2001WS, PCTEOLCRSWS, PCTEOLFINEWS, PCTEXTRUVOLWS, PCTFRSTLOSS2002WS, PCTGLACLAKECRSWS, PCTGLACLAKEFINEWS, PCTGLACTILCRSWS, PCTGRS2001WS, PCTHBWET2001WS, PCTICE2001WS, PCTIMP2001WS, PCTINCVEGRESP2002WS, PCTNONAGINTRODMANAGVEGWS, PCTOW2001WS, PCTSALLAKEWS, PCTSHRB2001WS, PCTURBHI2001WS, PCTURBLO2001WS, PCTURBOP2001WS, PCTWATERWS, PESTIC1997WS, POPDEN2010WS, PRECIP9120WS, RCKDEPWS, RDCRSSLPWTDWS, RDCRSWS, RDDENSWS, ROCKNWS, SANDWS, SEPTICWS, STRMPOW_CAT, SUPERFUNDDENSWS, SW_FLUXWS, SWS, TMAX9120WS, TRIDENSWS, WATERINPUTWS, WETINDEXWS, WETTEDWIDTH, WTDEPWS, WWTPALLDENSWS</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="str">
+        <f>_xlfn.TEXTJOIN(", ", TRUE, A1:A71)</f>
+        <v>BFIWS, CANALDENSWS, CLAYWS, COMPSTRGTHWS, DAMNRMSTORWS, ELEVWS, FE2O3WS, FERTWS, HYDRLCONDWS, K2OWS, KFFACTWS, MINEDENSWS, MSST2008, NANIWS, NHD_pSLOPE, NPDESDENSWS, NWS, OMWS, P2O5WS, PCT_EROD, PCTAGDRAINAGEWS, PCTALKINTRUVOLWS, PCTALLUVCOASTWS, PCTBL2001WS, PCTBURNAREA2002WS, PCTCARBRESIDWS, PCTCOLLUVSEDWS, PCTCONIF2001WS, PCTCROP2001WS, PCTDECID2001WS, PCTEOLFINEWS, PCTEXTRUVOLWS, PCTFRSTLOSS2002WS, PCTGLACLAKECRSWS, PCTGLACLAKEFINEWS, PCTGLACTILCRSWS, PCTGRS2001WS, PCTHAY2001WS, PCTHBWET2001WS, PCTICE2001WS, PCTIMP2001WS, PCTINCVEGRESP2002WS, PCTNONAGINTRODMANAGVEGWS, PCTOW2001WS, PCTSALLAKEWS, PCTSHRB2001WS, PCTURBHI2001WS, PCTURBLO2001WS, PCTURBOP2001WS, PCTWATERWS, PCTWDWET2001WS, PESTIC1997WS, POPDEN2010WS, PRECIP_MINUS_EVTWS, RCKDEPWS, RDCRSSLPWTDWS, RDCRSWS, RDDENSWS, ROCKNWS, SANDWS, SEPTICWS, STRMPOW_CAT, SUPERFUNDDENSWS, SW_FLUXWS, SWS, TMAX9120WS, TRIDENSWS, WETINDEXWS, WTDEPWS, WWTPALLDENSWS, WWTPMAJORDENSWS</v>
       </c>
     </row>
   </sheetData>

</xml_diff>